<commit_message>
implemented hashing with salt
</commit_message>
<xml_diff>
--- a/xlsxFiles/Time table 1.xlsx
+++ b/xlsxFiles/Time table 1.xlsx
@@ -43,7 +43,7 @@
       <sz val="16"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -58,26 +58,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCCCFF"/>
-        <bgColor rgb="00CCCCFF"/>
+        <fgColor rgb="00FFCCE5"/>
+        <bgColor rgb="00FFCCE5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF99FF"/>
-        <bgColor rgb="00FF99FF"/>
+        <fgColor rgb="00CCFFE5"/>
+        <bgColor rgb="00CCFFE5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E5FFCC"/>
-        <bgColor rgb="00E5FFCC"/>
+        <fgColor rgb="00FFCCFF"/>
+        <bgColor rgb="00FFCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFF99"/>
-        <bgColor rgb="00CCFF99"/>
+        <fgColor rgb="00CC99FF"/>
+        <bgColor rgb="00CC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009999FF"/>
+        <bgColor rgb="009999FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCFF"/>
+        <bgColor rgb="00CCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -93,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -102,16 +114,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -610,6 +628,18 @@
           <t>11:00</t>
         </is>
       </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>MONDAY CLASS 2
+11:00-12:30</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr">
+        <is>
+          <t>TESTING N2
+11:00-12:30</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
@@ -652,7 +682,7 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="C18" s="6" t="inlineStr">
+      <c r="C18" s="8" t="inlineStr">
         <is>
           <t>PHYSICS II
 14:00-15:30</t>
@@ -700,7 +730,7 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="F24" s="7" t="inlineStr">
+      <c r="F24" s="9" t="inlineStr">
         <is>
           <t>ECOLOGY
 17:00-19:00</t>
@@ -806,7 +836,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -816,6 +846,8 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="H12:H14"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C18:C20"/>

</xml_diff>